<commit_message>
I'm haeul. This is the Testing(commit)
</commit_message>
<xml_diff>
--- a/Recommand_app/Preferance_Data.xlsx
+++ b/Recommand_app/Preferance_Data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Desktop/Imagic_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harryn\Desktop\Git_hub\Imagic\Recommand_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="28800" windowHeight="16464"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -366,7 +366,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -680,28 +680,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P266"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:M208"/>
+    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
+      <selection activeCell="M263" sqref="M263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" customWidth="1"/>
+    <col min="6" max="6" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.6640625" style="8"/>
-    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,7 +746,7 @@
       </c>
       <c r="P1" s="9"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -793,7 +793,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -840,7 +840,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -887,7 +887,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -934,7 +934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -981,7 +981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>1</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -2203,7 +2203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>0</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>0</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>0</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>0</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>0</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>0</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>0</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>1</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>0</v>
       </c>
@@ -2718,7 +2718,7 @@
       </c>
       <c r="P43" s="5"/>
     </row>
-    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>0</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>1</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>1</v>
       </c>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>0</v>
       </c>
@@ -2943,7 +2943,7 @@
       </c>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>0</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1</v>
       </c>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>0</v>
       </c>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>0</v>
       </c>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>0</v>
       </c>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>0</v>
       </c>
@@ -3195,7 +3195,7 @@
       </c>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>1</v>
       </c>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>0</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>0</v>
       </c>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>1</v>
       </c>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>0</v>
       </c>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>0</v>
       </c>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>1</v>
       </c>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>1</v>
       </c>
@@ -3531,7 +3531,7 @@
       </c>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1</v>
       </c>
@@ -3573,7 +3573,7 @@
       </c>
       <c r="P63" s="1"/>
     </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>0</v>
       </c>
@@ -3615,7 +3615,7 @@
       </c>
       <c r="P64" s="1"/>
     </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>0</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="P65" s="1"/>
     </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>0</v>
       </c>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="P66" s="1"/>
     </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>0</v>
       </c>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>1</v>
       </c>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="P68" s="1"/>
     </row>
-    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>0</v>
       </c>
@@ -3825,7 +3825,7 @@
       </c>
       <c r="P69" s="1"/>
     </row>
-    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>1</v>
       </c>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="P70" s="1"/>
     </row>
-    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>0</v>
       </c>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="P71" s="1"/>
     </row>
-    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>0</v>
       </c>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="P72" s="1"/>
     </row>
-    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>0</v>
       </c>
@@ -3993,7 +3993,7 @@
       </c>
       <c r="P73" s="1"/>
     </row>
-    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>1</v>
       </c>
@@ -4035,7 +4035,7 @@
       </c>
       <c r="P74" s="1"/>
     </row>
-    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>0</v>
       </c>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="P75" s="1"/>
     </row>
-    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>0</v>
       </c>
@@ -4119,7 +4119,7 @@
       </c>
       <c r="P76" s="1"/>
     </row>
-    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>1</v>
       </c>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="P77" s="1"/>
     </row>
-    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>1</v>
       </c>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>0</v>
       </c>
@@ -4245,7 +4245,7 @@
       </c>
       <c r="P79" s="1"/>
     </row>
-    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>1</v>
       </c>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="P80" s="1"/>
     </row>
-    <row r="81" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>1</v>
       </c>
@@ -4329,7 +4329,7 @@
       </c>
       <c r="P81" s="1"/>
     </row>
-    <row r="82" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>0</v>
       </c>
@@ -4371,7 +4371,7 @@
       </c>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>0</v>
       </c>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="P83" s="1"/>
     </row>
-    <row r="84" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>0</v>
       </c>
@@ -4455,7 +4455,7 @@
       </c>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>0</v>
       </c>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="P85" s="1"/>
     </row>
-    <row r="86" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>0</v>
       </c>
@@ -4539,7 +4539,7 @@
       </c>
       <c r="P86" s="1"/>
     </row>
-    <row r="87" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>1</v>
       </c>
@@ -4581,7 +4581,7 @@
       </c>
       <c r="P87" s="1"/>
     </row>
-    <row r="88" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>0</v>
       </c>
@@ -4623,7 +4623,7 @@
       </c>
       <c r="P88" s="1"/>
     </row>
-    <row r="89" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>0</v>
       </c>
@@ -4665,7 +4665,7 @@
       </c>
       <c r="P89" s="1"/>
     </row>
-    <row r="90" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>1</v>
       </c>
@@ -4704,7 +4704,7 @@
       </c>
       <c r="P90" s="1"/>
     </row>
-    <row r="91" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>0</v>
       </c>
@@ -4746,7 +4746,7 @@
       </c>
       <c r="P91" s="1"/>
     </row>
-    <row r="92" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>0</v>
       </c>
@@ -4788,7 +4788,7 @@
       </c>
       <c r="P92" s="1"/>
     </row>
-    <row r="93" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>0</v>
       </c>
@@ -4830,7 +4830,7 @@
       </c>
       <c r="P93" s="1"/>
     </row>
-    <row r="94" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>0</v>
       </c>
@@ -4872,7 +4872,7 @@
       </c>
       <c r="P94" s="1"/>
     </row>
-    <row r="95" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>0</v>
       </c>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>1</v>
       </c>
@@ -4956,7 +4956,7 @@
       </c>
       <c r="P96" s="1"/>
     </row>
-    <row r="97" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>0</v>
       </c>
@@ -4998,7 +4998,7 @@
       </c>
       <c r="P97" s="1"/>
     </row>
-    <row r="98" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>1</v>
       </c>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="P98" s="1"/>
     </row>
-    <row r="99" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>1</v>
       </c>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="P99" s="1"/>
     </row>
-    <row r="100" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>0</v>
       </c>
@@ -5124,7 +5124,7 @@
       </c>
       <c r="P100" s="1"/>
     </row>
-    <row r="101" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>0</v>
       </c>
@@ -5166,7 +5166,7 @@
       </c>
       <c r="P101" s="1"/>
     </row>
-    <row r="102" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>0</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
       <c r="P102" s="1"/>
     </row>
-    <row r="103" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>1</v>
       </c>
@@ -5250,7 +5250,7 @@
       </c>
       <c r="P103" s="1"/>
     </row>
-    <row r="104" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>0</v>
       </c>
@@ -5292,7 +5292,7 @@
       </c>
       <c r="P104" s="1"/>
     </row>
-    <row r="105" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>1</v>
       </c>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="P105" s="1"/>
     </row>
-    <row r="106" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>0</v>
       </c>
@@ -5376,7 +5376,7 @@
       </c>
       <c r="P106" s="1"/>
     </row>
-    <row r="107" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>1</v>
       </c>
@@ -5418,7 +5418,7 @@
       </c>
       <c r="P107" s="1"/>
     </row>
-    <row r="108" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>1</v>
       </c>
@@ -5460,7 +5460,7 @@
       </c>
       <c r="P108" s="1"/>
     </row>
-    <row r="109" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>0</v>
       </c>
@@ -5502,7 +5502,7 @@
       </c>
       <c r="P109" s="1"/>
     </row>
-    <row r="110" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>0</v>
       </c>
@@ -5544,7 +5544,7 @@
       </c>
       <c r="P110" s="1"/>
     </row>
-    <row r="111" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>0</v>
       </c>
@@ -5586,7 +5586,7 @@
       </c>
       <c r="P111" s="1"/>
     </row>
-    <row r="112" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>1</v>
       </c>
@@ -5628,7 +5628,7 @@
       </c>
       <c r="P112" s="1"/>
     </row>
-    <row r="113" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>1</v>
       </c>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="P113" s="1"/>
     </row>
-    <row r="114" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>1</v>
       </c>
@@ -5712,7 +5712,7 @@
       </c>
       <c r="P114" s="1"/>
     </row>
-    <row r="115" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>0</v>
       </c>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="P115" s="1"/>
     </row>
-    <row r="116" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>0</v>
       </c>
@@ -5796,7 +5796,7 @@
       </c>
       <c r="P116" s="1"/>
     </row>
-    <row r="117" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>0</v>
       </c>
@@ -5838,7 +5838,7 @@
       </c>
       <c r="P117" s="1"/>
     </row>
-    <row r="118" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>0</v>
       </c>
@@ -5880,7 +5880,7 @@
       </c>
       <c r="P118" s="1"/>
     </row>
-    <row r="119" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>0</v>
       </c>
@@ -5922,7 +5922,7 @@
       </c>
       <c r="P119" s="1"/>
     </row>
-    <row r="120" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>1</v>
       </c>
@@ -5964,7 +5964,7 @@
       </c>
       <c r="P120" s="1"/>
     </row>
-    <row r="121" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>1</v>
       </c>
@@ -6006,7 +6006,7 @@
       </c>
       <c r="P121" s="1"/>
     </row>
-    <row r="122" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>0</v>
       </c>
@@ -6048,7 +6048,7 @@
       </c>
       <c r="P122" s="1"/>
     </row>
-    <row r="123" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>0</v>
       </c>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="P123" s="1"/>
     </row>
-    <row r="124" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>1</v>
       </c>
@@ -6132,7 +6132,7 @@
       </c>
       <c r="P124" s="1"/>
     </row>
-    <row r="125" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>0</v>
       </c>
@@ -6174,7 +6174,7 @@
       </c>
       <c r="P125" s="1"/>
     </row>
-    <row r="126" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>1</v>
       </c>
@@ -6216,7 +6216,7 @@
       </c>
       <c r="P126" s="1"/>
     </row>
-    <row r="127" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>0</v>
       </c>
@@ -6258,7 +6258,7 @@
       </c>
       <c r="P127" s="1"/>
     </row>
-    <row r="128" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>1</v>
       </c>
@@ -6300,7 +6300,7 @@
       </c>
       <c r="P128" s="1"/>
     </row>
-    <row r="129" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>1</v>
       </c>
@@ -6342,7 +6342,7 @@
       </c>
       <c r="P129" s="1"/>
     </row>
-    <row r="130" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>0</v>
       </c>
@@ -6384,7 +6384,7 @@
       </c>
       <c r="P130" s="1"/>
     </row>
-    <row r="131" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>0</v>
       </c>
@@ -6426,7 +6426,7 @@
       </c>
       <c r="P131" s="1"/>
     </row>
-    <row r="132" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>0</v>
       </c>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="P132" s="1"/>
     </row>
-    <row r="133" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>1</v>
       </c>
@@ -6510,7 +6510,7 @@
       </c>
       <c r="P133" s="1"/>
     </row>
-    <row r="134" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>0</v>
       </c>
@@ -6552,7 +6552,7 @@
       </c>
       <c r="P134" s="1"/>
     </row>
-    <row r="135" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>0</v>
       </c>
@@ -6594,7 +6594,7 @@
       </c>
       <c r="P135" s="1"/>
     </row>
-    <row r="136" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>0</v>
       </c>
@@ -6636,7 +6636,7 @@
       </c>
       <c r="P136" s="1"/>
     </row>
-    <row r="137" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>0</v>
       </c>
@@ -6678,7 +6678,7 @@
       </c>
       <c r="P137" s="1"/>
     </row>
-    <row r="138" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>0</v>
       </c>
@@ -6720,7 +6720,7 @@
       </c>
       <c r="P138" s="1"/>
     </row>
-    <row r="139" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>1</v>
       </c>
@@ -6762,7 +6762,7 @@
       </c>
       <c r="P139" s="1"/>
     </row>
-    <row r="140" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>1</v>
       </c>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="P140" s="1"/>
     </row>
-    <row r="141" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>1</v>
       </c>
@@ -6846,7 +6846,7 @@
       </c>
       <c r="P141" s="1"/>
     </row>
-    <row r="142" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>0</v>
       </c>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="P142" s="1"/>
     </row>
-    <row r="143" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>0</v>
       </c>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="P143" s="1"/>
     </row>
-    <row r="144" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>0</v>
       </c>
@@ -6969,7 +6969,7 @@
       </c>
       <c r="P144" s="1"/>
     </row>
-    <row r="145" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>0</v>
       </c>
@@ -7011,7 +7011,7 @@
       </c>
       <c r="P145" s="1"/>
     </row>
-    <row r="146" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>0</v>
       </c>
@@ -7053,7 +7053,7 @@
       </c>
       <c r="P146" s="1"/>
     </row>
-    <row r="147" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>1</v>
       </c>
@@ -7095,7 +7095,7 @@
       </c>
       <c r="P147" s="1"/>
     </row>
-    <row r="148" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>1</v>
       </c>
@@ -7137,7 +7137,7 @@
       </c>
       <c r="P148" s="1"/>
     </row>
-    <row r="149" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>1</v>
       </c>
@@ -7179,7 +7179,7 @@
       </c>
       <c r="P149" s="1"/>
     </row>
-    <row r="150" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>1</v>
       </c>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="P150" s="1"/>
     </row>
-    <row r="151" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>0</v>
       </c>
@@ -7263,7 +7263,7 @@
       </c>
       <c r="P151" s="1"/>
     </row>
-    <row r="152" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>0</v>
       </c>
@@ -7305,7 +7305,7 @@
       </c>
       <c r="P152" s="1"/>
     </row>
-    <row r="153" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>0</v>
       </c>
@@ -7347,7 +7347,7 @@
       </c>
       <c r="P153" s="1"/>
     </row>
-    <row r="154" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>0</v>
       </c>
@@ -7389,7 +7389,7 @@
       </c>
       <c r="P154" s="1"/>
     </row>
-    <row r="155" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>0</v>
       </c>
@@ -7431,7 +7431,7 @@
       </c>
       <c r="P155" s="1"/>
     </row>
-    <row r="156" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>0</v>
       </c>
@@ -7473,7 +7473,7 @@
       </c>
       <c r="P156" s="1"/>
     </row>
-    <row r="157" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>1</v>
       </c>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="P157" s="1"/>
     </row>
-    <row r="158" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>1</v>
       </c>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="P158" s="1"/>
     </row>
-    <row r="159" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>1</v>
       </c>
@@ -7599,7 +7599,7 @@
       </c>
       <c r="P159" s="1"/>
     </row>
-    <row r="160" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>1</v>
       </c>
@@ -7641,7 +7641,7 @@
       </c>
       <c r="P160" s="1"/>
     </row>
-    <row r="161" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>0</v>
       </c>
@@ -7683,7 +7683,7 @@
       </c>
       <c r="P161" s="1"/>
     </row>
-    <row r="162" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>0</v>
       </c>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="P162" s="1"/>
     </row>
-    <row r="163" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>0</v>
       </c>
@@ -7767,7 +7767,7 @@
       </c>
       <c r="P163" s="1"/>
     </row>
-    <row r="164" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>0</v>
       </c>
@@ -7809,7 +7809,7 @@
       </c>
       <c r="P164" s="1"/>
     </row>
-    <row r="165" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>0</v>
       </c>
@@ -7851,7 +7851,7 @@
       </c>
       <c r="P165" s="1"/>
     </row>
-    <row r="166" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>1</v>
       </c>
@@ -7893,7 +7893,7 @@
       </c>
       <c r="P166" s="1"/>
     </row>
-    <row r="167" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>0</v>
       </c>
@@ -7935,7 +7935,7 @@
       </c>
       <c r="P167" s="1"/>
     </row>
-    <row r="168" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>0</v>
       </c>
@@ -7977,7 +7977,7 @@
       </c>
       <c r="P168" s="1"/>
     </row>
-    <row r="169" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>0</v>
       </c>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="P169" s="1"/>
     </row>
-    <row r="170" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>0</v>
       </c>
@@ -8061,7 +8061,7 @@
       </c>
       <c r="P170" s="1"/>
     </row>
-    <row r="171" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>0</v>
       </c>
@@ -8103,7 +8103,7 @@
       </c>
       <c r="P171" s="1"/>
     </row>
-    <row r="172" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>0</v>
       </c>
@@ -8145,7 +8145,7 @@
       </c>
       <c r="P172" s="1"/>
     </row>
-    <row r="173" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>0</v>
       </c>
@@ -8187,7 +8187,7 @@
       </c>
       <c r="P173" s="1"/>
     </row>
-    <row r="174" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>0</v>
       </c>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="P174" s="1"/>
     </row>
-    <row r="175" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>0</v>
       </c>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="P175" s="1"/>
     </row>
-    <row r="176" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>0</v>
       </c>
@@ -8313,7 +8313,7 @@
       </c>
       <c r="P176" s="1"/>
     </row>
-    <row r="177" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>0</v>
       </c>
@@ -8355,7 +8355,7 @@
       </c>
       <c r="P177" s="1"/>
     </row>
-    <row r="178" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>1</v>
       </c>
@@ -8397,7 +8397,7 @@
       </c>
       <c r="P178" s="1"/>
     </row>
-    <row r="179" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>0</v>
       </c>
@@ -8439,7 +8439,7 @@
       </c>
       <c r="P179" s="1"/>
     </row>
-    <row r="180" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>1</v>
       </c>
@@ -8481,7 +8481,7 @@
       </c>
       <c r="P180" s="1"/>
     </row>
-    <row r="181" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>0</v>
       </c>
@@ -8523,7 +8523,7 @@
       </c>
       <c r="P181" s="1"/>
     </row>
-    <row r="182" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>0</v>
       </c>
@@ -8565,7 +8565,7 @@
       </c>
       <c r="P182" s="1"/>
     </row>
-    <row r="183" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>0</v>
       </c>
@@ -8607,7 +8607,7 @@
       </c>
       <c r="P183" s="1"/>
     </row>
-    <row r="184" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>0</v>
       </c>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="P184" s="1"/>
     </row>
-    <row r="185" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>0</v>
       </c>
@@ -8691,7 +8691,7 @@
       </c>
       <c r="P185" s="1"/>
     </row>
-    <row r="186" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>0</v>
       </c>
@@ -8733,7 +8733,7 @@
       </c>
       <c r="P186" s="1"/>
     </row>
-    <row r="187" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>0</v>
       </c>
@@ -8775,7 +8775,7 @@
       </c>
       <c r="P187" s="1"/>
     </row>
-    <row r="188" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>0</v>
       </c>
@@ -8817,7 +8817,7 @@
       </c>
       <c r="P188" s="1"/>
     </row>
-    <row r="189" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>0</v>
       </c>
@@ -8859,7 +8859,7 @@
       </c>
       <c r="P189" s="1"/>
     </row>
-    <row r="190" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>0</v>
       </c>
@@ -8901,7 +8901,7 @@
       </c>
       <c r="P190" s="1"/>
     </row>
-    <row r="191" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>0</v>
       </c>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="P191" s="1"/>
     </row>
-    <row r="192" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>1</v>
       </c>
@@ -8985,7 +8985,7 @@
       </c>
       <c r="P192" s="1"/>
     </row>
-    <row r="193" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>1</v>
       </c>
@@ -9027,7 +9027,7 @@
       </c>
       <c r="P193" s="1"/>
     </row>
-    <row r="194" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>1</v>
       </c>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="P194" s="1"/>
     </row>
-    <row r="195" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>1</v>
       </c>
@@ -9111,7 +9111,7 @@
       </c>
       <c r="P195" s="1"/>
     </row>
-    <row r="196" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>0</v>
       </c>
@@ -9153,7 +9153,7 @@
       </c>
       <c r="P196" s="1"/>
     </row>
-    <row r="197" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>0</v>
       </c>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="P197" s="1"/>
     </row>
-    <row r="198" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>0</v>
       </c>
@@ -9237,7 +9237,7 @@
       </c>
       <c r="P198" s="1"/>
     </row>
-    <row r="199" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>0</v>
       </c>
@@ -9279,7 +9279,7 @@
       </c>
       <c r="P199" s="1"/>
     </row>
-    <row r="200" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>0</v>
       </c>
@@ -9321,7 +9321,7 @@
       </c>
       <c r="P200" s="1"/>
     </row>
-    <row r="201" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>0</v>
       </c>
@@ -9363,7 +9363,7 @@
       </c>
       <c r="P201" s="1"/>
     </row>
-    <row r="202" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>0</v>
       </c>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="P202" s="1"/>
     </row>
-    <row r="203" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>1</v>
       </c>
@@ -9447,7 +9447,7 @@
       </c>
       <c r="P203" s="1"/>
     </row>
-    <row r="204" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>1</v>
       </c>
@@ -9489,7 +9489,7 @@
       </c>
       <c r="P204" s="1"/>
     </row>
-    <row r="205" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>0</v>
       </c>
@@ -9531,7 +9531,7 @@
       </c>
       <c r="P205" s="1"/>
     </row>
-    <row r="206" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>1</v>
       </c>
@@ -9573,7 +9573,7 @@
       </c>
       <c r="P206" s="1"/>
     </row>
-    <row r="207" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>0</v>
       </c>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="P207" s="1"/>
     </row>
-    <row r="208" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>0</v>
       </c>
@@ -9657,7 +9657,7 @@
       </c>
       <c r="P208" s="1"/>
     </row>
-    <row r="209" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>0</v>
       </c>
@@ -9697,7 +9697,7 @@
       <c r="M209" s="1"/>
       <c r="P209" s="1"/>
     </row>
-    <row r="210" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>1</v>
       </c>
@@ -9737,7 +9737,7 @@
       <c r="M210" s="1"/>
       <c r="P210" s="1"/>
     </row>
-    <row r="211" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>1</v>
       </c>
@@ -9777,7 +9777,7 @@
       <c r="M211" s="1"/>
       <c r="P211" s="1"/>
     </row>
-    <row r="212" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>0</v>
       </c>
@@ -9817,7 +9817,7 @@
       <c r="M212" s="1"/>
       <c r="P212" s="1"/>
     </row>
-    <row r="213" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>0</v>
       </c>
@@ -9857,7 +9857,7 @@
       <c r="M213" s="1"/>
       <c r="P213" s="1"/>
     </row>
-    <row r="214" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>0</v>
       </c>
@@ -9897,7 +9897,7 @@
       <c r="M214" s="1"/>
       <c r="P214" s="1"/>
     </row>
-    <row r="215" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>0</v>
       </c>
@@ -9937,7 +9937,7 @@
       <c r="M215" s="1"/>
       <c r="P215" s="1"/>
     </row>
-    <row r="216" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>0</v>
       </c>
@@ -9977,7 +9977,7 @@
       <c r="M216" s="1"/>
       <c r="P216" s="1"/>
     </row>
-    <row r="217" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>0</v>
       </c>
@@ -10017,7 +10017,7 @@
       <c r="M217" s="1"/>
       <c r="P217" s="1"/>
     </row>
-    <row r="218" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>0</v>
       </c>
@@ -10057,7 +10057,7 @@
       <c r="M218" s="1"/>
       <c r="P218" s="1"/>
     </row>
-    <row r="219" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>0</v>
       </c>
@@ -10097,7 +10097,7 @@
       <c r="M219" s="1"/>
       <c r="P219" s="1"/>
     </row>
-    <row r="220" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>0</v>
       </c>
@@ -10137,7 +10137,7 @@
       <c r="M220" s="1"/>
       <c r="P220" s="1"/>
     </row>
-    <row r="221" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>0</v>
       </c>
@@ -10177,7 +10177,7 @@
       <c r="M221" s="1"/>
       <c r="P221" s="1"/>
     </row>
-    <row r="222" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>0</v>
       </c>
@@ -10216,7 +10216,7 @@
       </c>
       <c r="P222" s="1"/>
     </row>
-    <row r="223" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>0</v>
       </c>
@@ -10255,7 +10255,7 @@
       </c>
       <c r="P223" s="1"/>
     </row>
-    <row r="224" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>0</v>
       </c>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="P224" s="1"/>
     </row>
-    <row r="225" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>0</v>
       </c>
@@ -10333,7 +10333,7 @@
       </c>
       <c r="P225" s="1"/>
     </row>
-    <row r="226" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>0</v>
       </c>
@@ -10372,7 +10372,7 @@
       </c>
       <c r="P226" s="1"/>
     </row>
-    <row r="227" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>0</v>
       </c>
@@ -10411,7 +10411,7 @@
       </c>
       <c r="P227" s="1"/>
     </row>
-    <row r="228" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>1</v>
       </c>
@@ -10450,7 +10450,7 @@
       </c>
       <c r="P228" s="1"/>
     </row>
-    <row r="229" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>0</v>
       </c>
@@ -10489,7 +10489,7 @@
       </c>
       <c r="P229" s="1"/>
     </row>
-    <row r="230" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>0</v>
       </c>
@@ -10528,7 +10528,7 @@
       </c>
       <c r="P230" s="1"/>
     </row>
-    <row r="231" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>1</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
       <c r="P231" s="1"/>
     </row>
-    <row r="232" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>0</v>
       </c>
@@ -10606,7 +10606,7 @@
       </c>
       <c r="P232" s="1"/>
     </row>
-    <row r="233" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>0</v>
       </c>
@@ -10645,7 +10645,7 @@
       </c>
       <c r="P233" s="1"/>
     </row>
-    <row r="234" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>0</v>
       </c>
@@ -10684,7 +10684,7 @@
       </c>
       <c r="P234" s="1"/>
     </row>
-    <row r="235" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>1</v>
       </c>
@@ -10723,7 +10723,7 @@
       </c>
       <c r="P235" s="1"/>
     </row>
-    <row r="236" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>1</v>
       </c>
@@ -10762,7 +10762,7 @@
       </c>
       <c r="P236" s="1"/>
     </row>
-    <row r="237" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>1</v>
       </c>
@@ -10801,7 +10801,7 @@
       </c>
       <c r="P237" s="1"/>
     </row>
-    <row r="238" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>0</v>
       </c>
@@ -10840,7 +10840,7 @@
       </c>
       <c r="P238" s="1"/>
     </row>
-    <row r="239" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>0</v>
       </c>
@@ -10879,7 +10879,7 @@
       </c>
       <c r="P239" s="1"/>
     </row>
-    <row r="240" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>1</v>
       </c>
@@ -10918,7 +10918,7 @@
       </c>
       <c r="P240" s="1"/>
     </row>
-    <row r="241" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>0</v>
       </c>
@@ -10957,7 +10957,7 @@
       </c>
       <c r="P241" s="1"/>
     </row>
-    <row r="242" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>1</v>
       </c>
@@ -10996,7 +10996,7 @@
       </c>
       <c r="P242" s="1"/>
     </row>
-    <row r="243" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>0</v>
       </c>
@@ -11035,7 +11035,7 @@
       </c>
       <c r="P243" s="1"/>
     </row>
-    <row r="244" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>0</v>
       </c>
@@ -11074,7 +11074,7 @@
       </c>
       <c r="P244" s="1"/>
     </row>
-    <row r="245" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>0</v>
       </c>
@@ -11113,7 +11113,7 @@
       </c>
       <c r="P245" s="1"/>
     </row>
-    <row r="246" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>0</v>
       </c>
@@ -11152,7 +11152,7 @@
       </c>
       <c r="P246" s="1"/>
     </row>
-    <row r="247" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>0</v>
       </c>
@@ -11191,7 +11191,7 @@
       </c>
       <c r="P247" s="1"/>
     </row>
-    <row r="248" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>0</v>
       </c>
@@ -11226,7 +11226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>0</v>
       </c>
@@ -11265,7 +11265,7 @@
       </c>
       <c r="P249" s="1"/>
     </row>
-    <row r="250" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>0</v>
       </c>
@@ -11304,7 +11304,7 @@
       </c>
       <c r="P250" s="1"/>
     </row>
-    <row r="251" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>1</v>
       </c>
@@ -11343,7 +11343,7 @@
       </c>
       <c r="P251" s="1"/>
     </row>
-    <row r="252" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>0</v>
       </c>
@@ -11382,7 +11382,7 @@
       </c>
       <c r="P252" s="1"/>
     </row>
-    <row r="253" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>0</v>
       </c>
@@ -11421,7 +11421,7 @@
       </c>
       <c r="P253" s="1"/>
     </row>
-    <row r="254" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>0</v>
       </c>
@@ -11460,7 +11460,7 @@
       </c>
       <c r="P254" s="1"/>
     </row>
-    <row r="255" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>0</v>
       </c>
@@ -11499,7 +11499,7 @@
       </c>
       <c r="P255" s="1"/>
     </row>
-    <row r="256" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>0</v>
       </c>
@@ -11538,7 +11538,7 @@
       </c>
       <c r="P256" s="1"/>
     </row>
-    <row r="257" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>1</v>
       </c>
@@ -11577,7 +11577,7 @@
       </c>
       <c r="P257" s="1"/>
     </row>
-    <row r="258" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>0</v>
       </c>
@@ -11616,7 +11616,7 @@
       </c>
       <c r="P258" s="1"/>
     </row>
-    <row r="259" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>0</v>
       </c>
@@ -11655,7 +11655,7 @@
       </c>
       <c r="P259" s="1"/>
     </row>
-    <row r="260" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>0</v>
       </c>
@@ -11694,7 +11694,7 @@
       </c>
       <c r="P260" s="1"/>
     </row>
-    <row r="261" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>0</v>
       </c>
@@ -11733,7 +11733,7 @@
       </c>
       <c r="P261" s="1"/>
     </row>
-    <row r="262" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>0</v>
       </c>
@@ -11772,7 +11772,7 @@
       </c>
       <c r="P262" s="1"/>
     </row>
-    <row r="263" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>0</v>
       </c>
@@ -11811,7 +11811,7 @@
       </c>
       <c r="P263" s="1"/>
     </row>
-    <row r="264" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>0</v>
       </c>
@@ -11850,8 +11850,45 @@
       </c>
       <c r="P264" s="1"/>
     </row>
-    <row r="265" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="266" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="265" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>0</v>
+      </c>
+      <c r="B265" s="1">
+        <v>0</v>
+      </c>
+      <c r="C265" s="1">
+        <v>0</v>
+      </c>
+      <c r="D265" s="1">
+        <v>1</v>
+      </c>
+      <c r="E265" s="1">
+        <v>1</v>
+      </c>
+      <c r="F265" s="1">
+        <v>1</v>
+      </c>
+      <c r="G265" s="1">
+        <v>0</v>
+      </c>
+      <c r="H265" s="1">
+        <v>1</v>
+      </c>
+      <c r="I265" s="1">
+        <v>0</v>
+      </c>
+      <c r="J265" s="1">
+        <v>0</v>
+      </c>
+      <c r="K265" s="1">
+        <v>0</v>
+      </c>
+      <c r="L265" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="M1:M266"/>
   <sortState ref="A2:M266">

</xml_diff>